<commit_message>
read data from file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,336 +441,1128 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>D1</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Tf1</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>idf</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Tf-idf1</t>
+          <t>Frekuensi kata</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>vladimir</t>
+          <t>markas</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
-        <v>1.301</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.783</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>putin</t>
+          <t>penyelidik</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.301</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.783</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>penjahat</t>
+          <t>pembunuhan</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.602</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>perang</t>
+          <t>anak</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.477</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.889</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>utama</t>
+          <t>kota</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.602</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>abad</t>
+          <t>aiide</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.602</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dugaan</t>
+          <t>lampu</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.602</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>kejahatan</t>
+          <t>neon</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.301</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.783</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>pemimpin</t>
+          <t>terkadang</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.602</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>rusia</t>
+          <t>berkedip</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.602</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ditujukkan</t>
+          <t>kedip</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.602</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ribuan</t>
+          <t>menerangi</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.602</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>targetnya</t>
+          <t>kertas</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.602</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>presiden</t>
+          <t>vertikal</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.602</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.602</v>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>dipajang</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>mencolok</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>sudut</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>pintu</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>masuk</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>aula</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>kantor</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>polisi</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>memandang</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>sakaguchi</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>menarik</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>kotak</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>rokok</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>kantong</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>jasnya</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>pagi</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>mayat</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>laki</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>berumur</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ditemukan</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>bersamaan</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>penyelidikan</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>memutuskan</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>membentuk</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>sore</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>harinya</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>diputuskan</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>menambah</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>anggota</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ajakan</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>bergabung</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>pria</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>buru</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>terletak</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>tokyo</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>barat</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>penduduk</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>jiwa</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>tempatnya</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>strategis</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>pergi</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>pusat</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>puluh</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>menit</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>kereta</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>menjadikan</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>terkenal</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>bed</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>town</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>orang</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>orangnya</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>tinggal</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>rumah</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>apartemen</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>cantik</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>perbelanjaan</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>praktis</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ditinggali</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>muda</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>tua</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>dibandingkan</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>harga</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>tanah</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>murah</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>memiliki</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>tamannya</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>taman</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>luas</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>berlarian</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>ceria</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>kucing</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>liar</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>berkeliaran</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>bebas</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>tenang</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>tingkat</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>kejahatan</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>rendah</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>daerah</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>dikenal</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>aman</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>tindak</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>kriminalitas</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>muncul</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>menghalanginya</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>perampokan</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>kekerasan</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>pembakaran</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>pemerkosaan</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>menculik</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>membunuhnya</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>syukurlah</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>jenazah</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>langsung</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>diliputi</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>suasana</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>mencekam</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>